<commit_message>
Final modification and results.
</commit_message>
<xml_diff>
--- a/Results/documentation of the RAs (in corpus for subject 070700).xlsx
+++ b/Results/documentation of the RAs (in corpus for subject 070700).xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -59,12 +56,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -556,8 +552,10 @@
           <t>海洋遥感</t>
         </is>
       </c>
-      <c r="H2" t="n">
-        <v>2017</v>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2017</t>
+        </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -641,8 +639,10 @@
           <t>海洋遥感</t>
         </is>
       </c>
-      <c r="H3" t="n">
-        <v>2013</v>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -727,8 +727,10 @@
           <t>海洋遥感</t>
         </is>
       </c>
-      <c r="H4" t="n">
-        <v>2013</v>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2013</t>
+        </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -812,8 +814,10 @@
           <t>海洋地质</t>
         </is>
       </c>
-      <c r="H5" s="2" t="n">
-        <v>43217</v>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2018-04-27 00:00:00</t>
+        </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -897,8 +901,10 @@
           <t>海洋地质</t>
         </is>
       </c>
-      <c r="H6" s="2" t="n">
-        <v>42572</v>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2016-07-21 00:00:00</t>
+        </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -982,8 +988,10 @@
           <t>海洋地质</t>
         </is>
       </c>
-      <c r="H7" s="2" t="n">
-        <v>41179</v>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>2012-09-27 00:00:00</t>
+        </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -1067,8 +1075,10 @@
           <t>海洋地质</t>
         </is>
       </c>
-      <c r="H8" t="n">
-        <v>2020</v>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -1152,8 +1162,10 @@
           <t>海洋地质</t>
         </is>
       </c>
-      <c r="H9" t="n">
-        <v>2019</v>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2019</t>
+        </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -1237,8 +1249,10 @@
           <t>海洋地质</t>
         </is>
       </c>
-      <c r="H10" t="n">
-        <v>2020</v>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -1322,8 +1336,10 @@
           <t>海洋技术</t>
         </is>
       </c>
-      <c r="H11" t="n">
-        <v>201409</v>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>201409</t>
+        </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -1407,8 +1423,10 @@
           <t>海洋技术</t>
         </is>
       </c>
-      <c r="H12" t="n">
-        <v>201808</v>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>201808</t>
+        </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -1492,8 +1510,10 @@
           <t>海洋技术</t>
         </is>
       </c>
-      <c r="H13" t="n">
-        <v>201910</v>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>201910</t>
+        </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -1577,8 +1597,10 @@
           <t>海洋技术</t>
         </is>
       </c>
-      <c r="H14" s="2" t="n">
-        <v>37165</v>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2001-10-01 00:00:00</t>
+        </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -1662,8 +1684,10 @@
           <t>海洋技术</t>
         </is>
       </c>
-      <c r="H15" s="2" t="n">
-        <v>36892</v>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2001-01-01 00:00:00</t>
+        </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -1747,8 +1771,10 @@
           <t>海洋技术</t>
         </is>
       </c>
-      <c r="H16" s="2" t="n">
-        <v>42257</v>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2015-09-10 00:00:00</t>
+        </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>

</xml_diff>